<commit_message>
Added actual Playwright project files
</commit_message>
<xml_diff>
--- a/src/test_data/CRM.xlsx
+++ b/src/test_data/CRM.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27518"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28110"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Documents\Ramrasad\qualizeal\playwright_demo\src\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="45" documentId="13_ncr:1_{4EE16FCC-9D86-4AA6-A067-7F5A0843827B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A2CD80D2-1CA8-4E2A-B3D2-DF62C883F154}"/>
+  <xr:revisionPtr revIDLastSave="49" documentId="13_ncr:1_{4EE16FCC-9D86-4AA6-A067-7F5A0843827B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{76D12EDE-B15E-4B0C-A055-20F7D116B1DB}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Companies" sheetId="1" r:id="rId1"/>
-    <sheet name="Contacts" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
+    <sheet name="Contacts" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="109">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -196,6 +197,110 @@
   </si>
   <si>
     <t>90000</t>
+  </si>
+  <si>
+    <t> </t>
+  </si>
+  <si>
+    <t>Auto</t>
+  </si>
+  <si>
+    <t>MO</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Create a reserve that </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>exceeds</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the user's authority</t>
+    </r>
+  </si>
+  <si>
+    <t>1) Reserve processes to "Pending Approval" status
+2) "Review and approve reserve change" activity generates to user's manager</t>
+  </si>
+  <si>
+    <t>AMO000070432</t>
+  </si>
+  <si>
+    <t>Passed</t>
+  </si>
+  <si>
+    <t>Roberto</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Create an automatic payment that </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>exceeds</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the user's authority</t>
+    </r>
+  </si>
+  <si>
+    <t>1) Payment processes to "Pending Approval" status
+2) "Review and approve new payment" activity generates to user's manager</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Create a Manual payment that </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>exceeds</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the user's authority</t>
+    </r>
   </si>
   <si>
     <t>First_name</t>
@@ -337,7 +442,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -371,6 +476,14 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="7">
@@ -452,7 +565,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -467,6 +580,10 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -750,7 +867,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -957,10 +1074,189 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE319A0F-B7E5-4DAD-A553-B78B9CB0E75B}">
+  <dimension ref="A1:P3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:P3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="1.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="2.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="58" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="31" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="16" width="1.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" ht="275.25">
+      <c r="A1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="G1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H1">
+        <v>3008153</v>
+      </c>
+      <c r="I1" t="s">
+        <v>59</v>
+      </c>
+      <c r="J1" s="13">
+        <v>45258</v>
+      </c>
+      <c r="K1" t="s">
+        <v>60</v>
+      </c>
+      <c r="L1" t="s">
+        <v>53</v>
+      </c>
+      <c r="M1" t="s">
+        <v>53</v>
+      </c>
+      <c r="N1" t="s">
+        <v>53</v>
+      </c>
+      <c r="O1" t="s">
+        <v>53</v>
+      </c>
+      <c r="P1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="275.25">
+      <c r="A2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="G2" t="s">
+        <v>58</v>
+      </c>
+      <c r="H2">
+        <v>3008153</v>
+      </c>
+      <c r="I2" t="s">
+        <v>59</v>
+      </c>
+      <c r="J2" s="13">
+        <v>45258</v>
+      </c>
+      <c r="K2" t="s">
+        <v>60</v>
+      </c>
+      <c r="L2" t="s">
+        <v>53</v>
+      </c>
+      <c r="M2" t="s">
+        <v>53</v>
+      </c>
+      <c r="N2" t="s">
+        <v>53</v>
+      </c>
+      <c r="O2" t="s">
+        <v>53</v>
+      </c>
+      <c r="P2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="275.25">
+      <c r="A3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" t="s">
+        <v>63</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="G3" t="s">
+        <v>58</v>
+      </c>
+      <c r="H3">
+        <v>3008153</v>
+      </c>
+      <c r="I3" t="s">
+        <v>59</v>
+      </c>
+      <c r="J3" s="13">
+        <v>45258</v>
+      </c>
+      <c r="K3" t="s">
+        <v>60</v>
+      </c>
+      <c r="L3" t="s">
+        <v>53</v>
+      </c>
+      <c r="M3" t="s">
+        <v>53</v>
+      </c>
+      <c r="N3" t="s">
+        <v>53</v>
+      </c>
+      <c r="O3" t="s">
+        <v>53</v>
+      </c>
+      <c r="P3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EAB8E4A-A4DD-418E-BDA0-6B511D42A51B}">
   <dimension ref="A1:Z3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
+    <sheetView topLeftCell="U1" workbookViewId="0">
       <selection activeCell="Z2" sqref="Z2:Z3"/>
     </sheetView>
   </sheetViews>
@@ -995,19 +1291,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>13</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>22</v>
@@ -1016,7 +1312,7 @@
         <v>11</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="J1" s="4" t="s">
         <v>20</v>
@@ -1025,40 +1321,40 @@
         <v>14</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="O1" s="4" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
       <c r="P1" s="4" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="Q1" s="4" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="R1" s="4" t="s">
-        <v>64</v>
+        <v>75</v>
       </c>
       <c r="S1" s="4" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="T1" s="4" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="U1" s="4" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="V1" s="4" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="W1" s="4" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="X1" s="4" t="s">
         <v>21</v>
@@ -1072,146 +1368,146 @@
     </row>
     <row r="2" spans="1:26" ht="15.75">
       <c r="A2" s="5" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>71</v>
+        <v>82</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>26</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>78</v>
+        <v>89</v>
       </c>
       <c r="K2" s="6"/>
       <c r="L2" s="6" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="M2" s="6"/>
       <c r="N2" s="6" t="s">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="O2" s="6" t="s">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="P2" s="6" t="s">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="Q2" s="8" t="s">
-        <v>83</v>
+        <v>94</v>
       </c>
       <c r="R2" s="6" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="S2" s="6" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="T2" s="8" t="s">
-        <v>85</v>
+        <v>96</v>
       </c>
       <c r="U2" s="6" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="V2" s="6" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="W2" s="6" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
       <c r="X2" s="6" t="s">
-        <v>89</v>
+        <v>100</v>
       </c>
       <c r="Y2" s="11"/>
       <c r="Z2" s="11" t="s">
-        <v>90</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="16.5">
       <c r="A3" s="10" t="s">
-        <v>91</v>
+        <v>102</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>92</v>
+        <v>103</v>
       </c>
       <c r="C3" s="11"/>
       <c r="D3" s="6" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="F3" s="6"/>
       <c r="G3" s="6" t="s">
-        <v>95</v>
+        <v>106</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>96</v>
+        <v>107</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>97</v>
+        <v>108</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>78</v>
+        <v>89</v>
       </c>
       <c r="K3" s="11"/>
       <c r="L3" s="6" t="s">
-        <v>89</v>
+        <v>100</v>
       </c>
       <c r="M3" s="11"/>
       <c r="N3" s="6" t="s">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="O3" s="6" t="s">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="P3" s="6" t="s">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="Q3" s="8" t="s">
-        <v>83</v>
+        <v>94</v>
       </c>
       <c r="R3" s="6" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="S3" s="6" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="T3" s="8" t="s">
-        <v>85</v>
+        <v>96</v>
       </c>
       <c r="U3" s="6" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="V3" s="6" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="W3" s="6" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
       <c r="X3" s="6" t="s">
-        <v>89</v>
+        <v>100</v>
       </c>
       <c r="Y3" s="11"/>
       <c r="Z3" s="11" t="s">
-        <v>90</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>